<commit_message>
Nhom 12 cap nhat
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Nhom12/Template_BangDanhGiaThanhVien.xlsx
+++ b/ProjectDocuments/Nhom12/Template_BangDanhGiaThanhVien.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>BẢNG ĐÁNH GIÁ THÀNH VIÊN</t>
   </si>
@@ -88,6 +88,36 @@
   </si>
   <si>
     <t>Phân công 7</t>
+  </si>
+  <si>
+    <t>0712110</t>
+  </si>
+  <si>
+    <t>0712127</t>
+  </si>
+  <si>
+    <t>0712129</t>
+  </si>
+  <si>
+    <t>0712138</t>
+  </si>
+  <si>
+    <t>0712325</t>
+  </si>
+  <si>
+    <t>Đoàn Nguyên Dương</t>
+  </si>
+  <si>
+    <t>Trần Đức Duy</t>
+  </si>
+  <si>
+    <t>Trịnh Khắc Duy</t>
+  </si>
+  <si>
+    <t>Nguyễn Việt Hằng</t>
+  </si>
+  <si>
+    <t>Trần Nam Phương</t>
   </si>
 </sst>
 </file>
@@ -98,28 +128,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -201,7 +231,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -245,6 +275,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -544,24 +575,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="11.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.09765625" style="1"/>
+    <col min="3" max="3" width="11.8984375" style="7" customWidth="1"/>
     <col min="4" max="4" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="11" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16" width="9.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="45.69921875" style="1" customWidth="1"/>
+    <col min="13" max="16" width="9.09765625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.296875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.09765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45.75">
+    <row r="1" spans="1:12" ht="46.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -578,7 +609,7 @@
     <row r="2" spans="1:12">
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:12" ht="40.5">
+    <row r="3" spans="1:12" ht="21">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -705,30 +736,66 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="C9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="17">
+        <v>1</v>
+      </c>
+      <c r="G9" s="17">
+        <v>1</v>
+      </c>
+      <c r="H9" s="17">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17">
+        <v>1</v>
+      </c>
+      <c r="J9" s="17">
+        <v>1</v>
+      </c>
+      <c r="K9" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="16"/>
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="C10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="17">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17">
+        <v>1</v>
+      </c>
+      <c r="H10" s="17">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17">
+        <v>1</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="17">
+        <v>1</v>
+      </c>
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12">
@@ -736,45 +803,99 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="C11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="17">
+        <v>1</v>
+      </c>
+      <c r="H11" s="17">
+        <v>1</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="K11" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="16"/>
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="C12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="17">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17">
+        <v>1</v>
+      </c>
+      <c r="H12" s="17">
+        <v>1</v>
+      </c>
+      <c r="I12" s="17">
+        <v>1</v>
+      </c>
+      <c r="J12" s="17">
+        <v>1</v>
+      </c>
+      <c r="K12" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="16"/>
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="C13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="17">
+        <v>1</v>
+      </c>
+      <c r="G13" s="17">
+        <v>1</v>
+      </c>
+      <c r="H13" s="17">
+        <v>1</v>
+      </c>
+      <c r="I13" s="17">
+        <v>1</v>
+      </c>
+      <c r="J13" s="17">
+        <v>1</v>
+      </c>
+      <c r="K13" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="14">
@@ -1047,7 +1168,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1059,7 +1180,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>